<commit_message>
Perbarui seluruh halaman HTML dan model prediksi
</commit_message>
<xml_diff>
--- a/Dataset_Gejala Ayam.xlsx
+++ b/Dataset_Gejala Ayam.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KULIAH\Semester 8\Tugas Akhir\Website\website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KULIAH\Semester 8\Tugas Akhir\Website\Website-MediChick\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -506,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI84" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AM102" sqref="AM102"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4528,7 +4528,7 @@
         <v>1</v>
       </c>
       <c r="K35" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L35" s="1">
         <v>0</v>
@@ -4760,7 +4760,7 @@
         <v>1</v>
       </c>
       <c r="K37" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L37" s="1">
         <v>0</v>
@@ -4876,7 +4876,7 @@
         <v>1</v>
       </c>
       <c r="K38" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L38" s="1">
         <v>0</v>
@@ -5108,7 +5108,7 @@
         <v>1</v>
       </c>
       <c r="K40" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L40" s="1">
         <v>0</v>
@@ -5456,7 +5456,7 @@
         <v>1</v>
       </c>
       <c r="K43" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L43" s="1">
         <v>0</v>

</xml_diff>